<commit_message>
added one more sheet
</commit_message>
<xml_diff>
--- a/online_course/source/module2/wallet.xlsx
+++ b/online_course/source/module2/wallet.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wallet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="squrs" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="123">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -383,6 +384,12 @@
   </si>
   <si>
     <t xml:space="preserve">2020-10-11 16:53:28.377359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sqr(x)</t>
   </si>
 </sst>
 </file>
@@ -398,6 +405,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -485,8 +493,8 @@
   </sheetPr>
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2222,4 +2230,201 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">A2*A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">A3*A3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">A4*A4</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">A5*A5</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">A6*A6</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">A7*A7</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">A8*A8</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">A9*A9</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">A10*A10</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">A11*A11</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">A12*A12</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">A13*A13</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">A14*A14</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">A15*A15</f>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">A16*A16</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">A17*A17</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">A18*A18</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">A19*A19</f>
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>